<commit_message>
ico and config for pre release
</commit_message>
<xml_diff>
--- a/doc/pert_manage.xlsx
+++ b/doc/pert_manage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs003_Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs003-Face-cognition-Sign-In-System\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0724BF-F9E0-4638-8019-9D9699BA2DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D223E2-80F0-4E02-B7E1-0E5B0459DC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22845" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,10 +133,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Expected time €</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>start_date(original)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,6 +192,18 @@
     <t>D,G,H,I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expected time (E)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -203,7 +211,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -254,8 +262,8 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2553,7 +2561,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
@@ -2698,6 +2706,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2721,7 +2730,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
@@ -2866,6 +2875,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2889,7 +2899,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
@@ -3034,6 +3044,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -3057,7 +3068,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
@@ -3202,6 +3213,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -3532,8 +3544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3544,7 +3556,7 @@
     <col min="4" max="4" width="20.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.875" style="6" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" customWidth="1"/>
     <col min="9" max="10" width="15.375" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
@@ -3584,8 +3596,8 @@
       <c r="F2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="5">
-        <f>ROUNDUP((D2+4*E2+F2)/6,0)</f>
+      <c r="G2" s="6">
+        <f>(D2+4*E2+F2)/6</f>
         <v>4</v>
       </c>
       <c r="H2" s="1">
@@ -3609,7 +3621,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1">
         <v>3</v>
@@ -3620,19 +3632,19 @@
       <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="G3" s="5">
-        <f>ROUNDUP((D3+4*E3+F3)/6,0)</f>
-        <v>3</v>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G11" si="1">(D3+4*E3+F3)/6</f>
+        <v>2.6666666666666665</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
       </c>
       <c r="I3" s="6">
-        <f t="shared" ref="I3:I11" si="1">POWER((F3-D3)/6,2)</f>
+        <f t="shared" ref="I3:I11" si="2">POWER((F3-D3)/6,2)</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="J3" s="6">
-        <f t="shared" ref="J3:J11" si="2">ABS((F3-D3)/6)</f>
+        <f t="shared" ref="J3:J11" si="3">ABS((F3-D3)/6)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -3645,7 +3657,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
@@ -3656,19 +3668,19 @@
       <c r="F4" s="1">
         <v>7</v>
       </c>
-      <c r="G4" s="5">
-        <f t="shared" ref="G4:G11" si="3">ROUNDUP((D4+4*E4+F4)/6,0)</f>
-        <v>4</v>
+      <c r="G4" s="6">
+        <f t="shared" si="1"/>
+        <v>3.8333333333333335</v>
       </c>
       <c r="H4" s="1">
         <v>6</v>
       </c>
       <c r="I4" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3681,7 +3693,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
@@ -3692,19 +3704,19 @@
       <c r="F5" s="1">
         <v>7</v>
       </c>
-      <c r="G5" s="5">
-        <f t="shared" si="3"/>
-        <v>6</v>
+      <c r="G5" s="6">
+        <f t="shared" si="1"/>
+        <v>5.833333333333333</v>
       </c>
       <c r="H5" s="1">
         <v>6</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="J5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3717,7 +3729,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1">
         <v>14</v>
@@ -3728,19 +3740,19 @@
       <c r="F6" s="1">
         <v>21</v>
       </c>
-      <c r="G6" s="5">
-        <f t="shared" si="3"/>
-        <v>18</v>
+      <c r="G6" s="6">
+        <f t="shared" si="1"/>
+        <v>17.833333333333332</v>
       </c>
       <c r="H6" s="1">
         <v>16</v>
       </c>
       <c r="I6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3611111111111114</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1666666666666667</v>
       </c>
     </row>
@@ -3764,19 +3776,19 @@
       <c r="F7" s="1">
         <v>21</v>
       </c>
-      <c r="G7" s="5">
-        <f t="shared" si="3"/>
-        <v>19</v>
+      <c r="G7" s="6">
+        <f t="shared" si="1"/>
+        <v>18.666666666666668</v>
       </c>
       <c r="H7" s="1">
         <v>10</v>
       </c>
       <c r="I7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3800,19 +3812,19 @@
       <c r="F8" s="1">
         <v>7</v>
       </c>
-      <c r="G8" s="5">
-        <f t="shared" si="3"/>
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H8" s="1">
         <v>5</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -3836,19 +3848,19 @@
       <c r="F9" s="1">
         <v>7</v>
       </c>
-      <c r="G9" s="5">
-        <f t="shared" si="3"/>
-        <v>6</v>
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>5.166666666666667</v>
       </c>
       <c r="H9" s="1">
         <v>5</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3872,19 +3884,19 @@
       <c r="F10" s="1">
         <v>10</v>
       </c>
-      <c r="G10" s="5">
-        <f t="shared" si="3"/>
-        <v>8</v>
+      <c r="G10" s="6">
+        <f t="shared" si="1"/>
+        <v>7.666666666666667</v>
       </c>
       <c r="H10" s="1">
         <v>5</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -3908,19 +3920,19 @@
       <c r="F11" s="1">
         <v>10</v>
       </c>
-      <c r="G11" s="5">
-        <f t="shared" si="3"/>
-        <v>8</v>
+      <c r="G11" s="6">
+        <f t="shared" si="1"/>
+        <v>7.166666666666667</v>
       </c>
       <c r="H11" s="1">
         <v>12</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69444444444444453</v>
       </c>
       <c r="J11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -3937,9 +3949,9 @@
         <f>SUM(F2:F11)</f>
         <v>100</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="6">
         <f>SUM(G2:G11)</f>
-        <v>81</v>
+        <v>77.833333333333329</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(H2:H11)</f>
@@ -3949,43 +3961,84 @@
         <f>SQRT(SUM(I2:I11))</f>
         <v>2.3392781412697001</v>
       </c>
-      <c r="J12" s="7"/>
+      <c r="J12" s="7">
+        <f>SQRT(I12)</f>
+        <v>1.529469888971241</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3">
+      <c r="C14" s="3">
         <v>0.68259999999999998</v>
+      </c>
+      <c r="D14" s="5">
+        <f>ROUNDUP(G12-J12,0)</f>
+        <v>77</v>
+      </c>
+      <c r="E14" s="5">
+        <f>ROUNDUP(G12+J12,0)</f>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3">
+      <c r="C15" s="3">
         <v>0.9546</v>
+      </c>
+      <c r="D15" s="1">
+        <f>ROUNDUP(G12-2*J12,0)</f>
+        <v>75</v>
+      </c>
+      <c r="E15" s="1">
+        <f>ROUNDUP(G12+2*J12,0)</f>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="3">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3">
         <v>0.99729999999999996</v>
       </c>
+      <c r="D16" s="1">
+        <f>ROUNDUP(G12-3*J12,0)</f>
+        <v>74</v>
+      </c>
+      <c r="E16" s="1">
+        <f>ROUNDUP(G12+3*J12,0)</f>
+        <v>83</v>
+      </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="3">
+      <c r="C17" s="3">
         <v>0.99990000000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <f>ROUNDUP(G12-6*J12,0)</f>
+        <v>69</v>
+      </c>
+      <c r="E17" s="1">
+        <f>ROUNDUP(G12+6*J12,0)</f>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -4000,7 +4053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F1006-280E-44A7-8D21-D4A9410363AC}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -4021,7 +4074,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -4078,7 +4131,7 @@
         <v>D</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4">
         <v>44465</v>
@@ -4185,52 +4238,52 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>